<commit_message>
Biblos - A28-D | Alfa L8.83.1
</commit_message>
<xml_diff>
--- a/vendor/phpoffice/phpspreadsheet/src/PhpSpreadsheet/Calculation/locale/Translations.xlsx
+++ b/vendor/phpoffice/phpspreadsheet/src/PhpSpreadsheet/Calculation/locale/Translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PHPOffice\PHPSpreadsheet\develop\src\PhpSpreadsheet\Calculation\locale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F14B4C-B7A9-4CCB-93EC-FA8A16A75332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48C1BC0-1CE1-483D-8D6D-B0314F47B0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4406" yWindow="1243" windowWidth="24685" windowHeight="16723" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7123" yWindow="2057" windowWidth="24686" windowHeight="16149" tabRatio="989" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Excel Localisation" sheetId="4" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8611" uniqueCount="6515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8630" uniqueCount="6535">
   <si>
     <t>SUBTOTAL</t>
   </si>
@@ -19614,13 +19614,73 @@
   </si>
   <si>
     <t>DIV0</t>
+  </si>
+  <si>
+    <t>ДОЛЛСША</t>
+  </si>
+  <si>
+    <t>ФИЛЬТР</t>
+  </si>
+  <si>
+    <t>СОРТ</t>
+  </si>
+  <si>
+    <t>СОРТПО</t>
+  </si>
+  <si>
+    <t>УНИК</t>
+  </si>
+  <si>
+    <t>ПРОСМОТРX</t>
+  </si>
+  <si>
+    <t>ПОИСКПОЗX</t>
+  </si>
+  <si>
+    <t>СЛУЧМАССИВ</t>
+  </si>
+  <si>
+    <t>ПОСЛЕДОВ</t>
+  </si>
+  <si>
+    <t>МАССИВВТЕКСТ</t>
+  </si>
+  <si>
+    <t>БДЦС</t>
+  </si>
+  <si>
+    <t>НАЙТИБ</t>
+  </si>
+  <si>
+    <t>ЛЕВБ</t>
+  </si>
+  <si>
+    <t>ДЛИНБ</t>
+  </si>
+  <si>
+    <t>ПСТРБ</t>
+  </si>
+  <si>
+    <t>ЗАМЕНИТЬБ</t>
+  </si>
+  <si>
+    <t>ПРАВБ</t>
+  </si>
+  <si>
+    <t>ПОИСКБ</t>
+  </si>
+  <si>
+    <t>ЗНАЧЕНИЕВТЕКСТ</t>
+  </si>
+  <si>
+    <t>ЕТАЙЦИФРЫ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -19632,12 +19692,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -19675,10 +19729,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -20037,11 +20091,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1A36666-6E7A-4A48-9C4E-B256160FF964}">
   <dimension ref="A1:AA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -20852,11 +20906,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31683534-79D8-42E0-A1E0-6E4CC43822BE}">
   <dimension ref="A1:R526"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="F435" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" sqref="A1:A3"/>
+      <selection pane="bottomRight" activeCell="G444" sqref="G444"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -20881,7 +20935,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -20937,7 +20991,7 @@
       </c>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="4"/>
+      <c r="A2" s="5"/>
       <c r="C2" s="2" t="s">
         <v>5768</v>
       </c>
@@ -20988,7 +21042,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A3" s="4"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="2" t="s">
         <v>2004</v>
       </c>
@@ -29304,6 +29358,9 @@
       <c r="B164" s="1" t="s">
         <v>6145</v>
       </c>
+      <c r="G164" s="1" t="s">
+        <v>6515</v>
+      </c>
     </row>
     <row r="165" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B165" s="1" t="s">
@@ -31713,6 +31770,9 @@
       <c r="B213" s="1" t="s">
         <v>6081</v>
       </c>
+      <c r="G213" s="1" t="s">
+        <v>6516</v>
+      </c>
     </row>
     <row r="214" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B214" s="1" t="s">
@@ -32355,12 +32415,18 @@
       <c r="B226" s="1" t="s">
         <v>6082</v>
       </c>
+      <c r="G226" s="1" t="s">
+        <v>6517</v>
+      </c>
     </row>
     <row r="227" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A227" s="2"/>
       <c r="B227" s="1" t="s">
         <v>6083</v>
       </c>
+      <c r="G227" s="1" t="s">
+        <v>6518</v>
+      </c>
     </row>
     <row r="228" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B228" s="1" t="s">
@@ -32420,6 +32486,9 @@
       <c r="B229" s="1" t="s">
         <v>6084</v>
       </c>
+      <c r="G229" s="1" t="s">
+        <v>6519</v>
+      </c>
     </row>
     <row r="230" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B230" s="1" t="s">
@@ -32479,12 +32548,18 @@
       <c r="B231" s="1" t="s">
         <v>6085</v>
       </c>
+      <c r="G231" s="1" t="s">
+        <v>6520</v>
+      </c>
     </row>
     <row r="232" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A232" s="2"/>
       <c r="B232" s="1" t="s">
         <v>6086</v>
       </c>
+      <c r="G232" s="1" t="s">
+        <v>6521</v>
+      </c>
     </row>
     <row r="233" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A233" s="2"/>
@@ -35351,6 +35426,9 @@
       <c r="B288" s="1" t="s">
         <v>6090</v>
       </c>
+      <c r="G288" s="1" t="s">
+        <v>6522</v>
+      </c>
     </row>
     <row r="289" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B289" s="1" t="s">
@@ -35871,6 +35949,9 @@
       <c r="B299" s="1" t="s">
         <v>6091</v>
       </c>
+      <c r="G299" s="1" t="s">
+        <v>6523</v>
+      </c>
     </row>
     <row r="300" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B300" s="1" t="s">
@@ -42721,17 +42802,20 @@
         <v>5911</v>
       </c>
     </row>
-    <row r="431" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B431" s="5" t="s">
+    <row r="431" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B431" s="4" t="s">
         <v>6092</v>
       </c>
-      <c r="R431" s="5" t="s">
+      <c r="R431" s="4" t="s">
         <v>6113</v>
       </c>
     </row>
-    <row r="432" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B432" s="5" t="s">
+    <row r="432" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B432" s="4" t="s">
         <v>6093</v>
+      </c>
+      <c r="G432" s="4" t="s">
+        <v>6524</v>
       </c>
     </row>
     <row r="433" spans="1:18" x14ac:dyDescent="0.4">
@@ -43004,6 +43088,9 @@
       <c r="B438" s="1" t="s">
         <v>6094</v>
       </c>
+      <c r="G438" s="1" t="s">
+        <v>6525</v>
+      </c>
     </row>
     <row r="439" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B439" s="1" t="s">
@@ -43169,6 +43256,9 @@
       <c r="B442" s="1" t="s">
         <v>6095</v>
       </c>
+      <c r="G442" s="1" t="s">
+        <v>6526</v>
+      </c>
     </row>
     <row r="443" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B443" s="1" t="s">
@@ -43235,7 +43325,7 @@
         <v>6190</v>
       </c>
       <c r="G444" s="1" t="s">
-        <v>6190</v>
+        <v>6534</v>
       </c>
       <c r="H444" s="1" t="s">
         <v>6191</v>
@@ -43323,6 +43413,9 @@
       <c r="B446" s="1" t="s">
         <v>6096</v>
       </c>
+      <c r="G446" s="1" t="s">
+        <v>6527</v>
+      </c>
     </row>
     <row r="447" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B447" s="1" t="s">
@@ -43382,6 +43475,9 @@
       <c r="B448" s="1" t="s">
         <v>6097</v>
       </c>
+      <c r="G448" s="1" t="s">
+        <v>6528</v>
+      </c>
     </row>
     <row r="449" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B449" s="1" t="s">
@@ -43494,6 +43590,9 @@
       <c r="B451" s="1" t="s">
         <v>6098</v>
       </c>
+      <c r="G451" s="1" t="s">
+        <v>6529</v>
+      </c>
     </row>
     <row r="452" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A452" s="2"/>
@@ -43743,6 +43842,9 @@
       <c r="B457" s="1" t="s">
         <v>6100</v>
       </c>
+      <c r="G457" s="1" t="s">
+        <v>6530</v>
+      </c>
     </row>
     <row r="458" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B458" s="1" t="s">
@@ -43855,6 +43957,9 @@
       <c r="B460" s="1" t="s">
         <v>6101</v>
       </c>
+      <c r="G460" s="1" t="s">
+        <v>6531</v>
+      </c>
     </row>
     <row r="461" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B461" s="1" t="s">
@@ -43914,6 +44019,9 @@
       <c r="B462" s="1" t="s">
         <v>6102</v>
       </c>
+      <c r="G462" s="1" t="s">
+        <v>6532</v>
+      </c>
     </row>
     <row r="463" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B463" s="1" t="s">
@@ -44576,6 +44684,9 @@
       <c r="A476" s="2"/>
       <c r="B476" s="1" t="s">
         <v>6103</v>
+      </c>
+      <c r="G476" s="1" t="s">
+        <v>6533</v>
       </c>
     </row>
     <row r="477" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">

</xml_diff>